<commit_message>
EPBDS-6561 Add cycled dependency on beans
--HG--
branch : 5.19.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.project/test-resources/classpath/multi1/datatypes.xlsx
+++ b/STUDIO/org.openl.rules.project/test-resources/classpath/multi1/datatypes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Datatype Person</t>
   </si>
@@ -41,6 +41,21 @@
   </si>
   <si>
     <t>com.example.beans.openl</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>adr</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>com.example.beans</t>
   </si>
 </sst>
 </file>
@@ -381,11 +396,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
@@ -437,6 +459,28 @@
       </c>
       <c r="D6" s="2"/>
     </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>